<commit_message>
added accounts test cases
</commit_message>
<xml_diff>
--- a/src/main/java/com/sf/qa/testdata/SFTestData.xlsx
+++ b/src/main/java/com/sf/qa/testdata/SFTestData.xlsx
@@ -5,15 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UdemyWS\SFTest\src\main\java\com\sf\qa\testdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\devendra_parate\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BABF578-061C-4344-9594-DFD1034F47FF}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82740F5E-674F-4AC8-AC49-11D31FF7E956}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{8329FF20-541C-4C8D-8267-D59AB2F4BA89}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{8329FF20-541C-4C8D-8267-D59AB2F4BA89}"/>
   </bookViews>
   <sheets>
     <sheet name="leads" sheetId="1" r:id="rId1"/>
+    <sheet name="accounts (2)" sheetId="4" r:id="rId2"/>
+    <sheet name="accounts" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -25,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="80">
   <si>
     <t>salutation</t>
   </si>
@@ -73,13 +75,205 @@
   </si>
   <si>
     <t>manoj</t>
+  </si>
+  <si>
+    <t>accountName</t>
+  </si>
+  <si>
+    <t>phone</t>
+  </si>
+  <si>
+    <t>website</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>ownership</t>
+  </si>
+  <si>
+    <t>industry</t>
+  </si>
+  <si>
+    <t>billingStreet</t>
+  </si>
+  <si>
+    <t>billingCity</t>
+  </si>
+  <si>
+    <t>billingZip</t>
+  </si>
+  <si>
+    <t>billingCountry</t>
+  </si>
+  <si>
+    <t>shippingStreet</t>
+  </si>
+  <si>
+    <t>shippingCity</t>
+  </si>
+  <si>
+    <t>shippingState</t>
+  </si>
+  <si>
+    <t>shippingZip</t>
+  </si>
+  <si>
+    <t>shippingCountry</t>
+  </si>
+  <si>
+    <t>billingState</t>
+  </si>
+  <si>
+    <t>active</t>
+  </si>
+  <si>
+    <t>rating</t>
+  </si>
+  <si>
+    <t>Hot</t>
+  </si>
+  <si>
+    <t>61 2 9876 5432</t>
+  </si>
+  <si>
+    <t>Customer - Direct</t>
+  </si>
+  <si>
+    <t>Private</t>
+  </si>
+  <si>
+    <t>Engineering</t>
+  </si>
+  <si>
+    <t>ABC Corp</t>
+  </si>
+  <si>
+    <t>www.abccorp.com</t>
+  </si>
+  <si>
+    <t>QLD</t>
+  </si>
+  <si>
+    <t>SA</t>
+  </si>
+  <si>
+    <t>WA</t>
+  </si>
+  <si>
+    <t>NSW</t>
+  </si>
+  <si>
+    <t>ACT</t>
+  </si>
+  <si>
+    <t>Brisbane</t>
+  </si>
+  <si>
+    <t>Whyalla</t>
+  </si>
+  <si>
+    <t>Perth</t>
+  </si>
+  <si>
+    <t>Sydney</t>
+  </si>
+  <si>
+    <t>‎Canberra</t>
+  </si>
+  <si>
+    <t>Australia</t>
+  </si>
+  <si>
+    <t>252 Wellington Rd</t>
+  </si>
+  <si>
+    <t>303 Adelaide St</t>
+  </si>
+  <si>
+    <t>48 Montague Rd</t>
+  </si>
+  <si>
+    <t>8 Edgar St</t>
+  </si>
+  <si>
+    <t>23 Wellington St</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>Consulting</t>
+  </si>
+  <si>
+    <t>Banking</t>
+  </si>
+  <si>
+    <t>Communications</t>
+  </si>
+  <si>
+    <t>Healthcare</t>
+  </si>
+  <si>
+    <t>Public</t>
+  </si>
+  <si>
+    <t>Other</t>
+  </si>
+  <si>
+    <t>Warm</t>
+  </si>
+  <si>
+    <t>Cold</t>
+  </si>
+  <si>
+    <t>62 2 9876 5433</t>
+  </si>
+  <si>
+    <t>63 2 9876 5434</t>
+  </si>
+  <si>
+    <t>64 2 9876 5435</t>
+  </si>
+  <si>
+    <t>65 2 9876 5436</t>
+  </si>
+  <si>
+    <t>Thechopark</t>
+  </si>
+  <si>
+    <t>www.technopark.com</t>
+  </si>
+  <si>
+    <t>Bank24</t>
+  </si>
+  <si>
+    <t>www.bank24.au.com</t>
+  </si>
+  <si>
+    <t>ConnectTelecomm</t>
+  </si>
+  <si>
+    <t>www.connecttelecom.com</t>
+  </si>
+  <si>
+    <t>AtService</t>
+  </si>
+  <si>
+    <t>www.atservice.au.com</t>
+  </si>
+  <si>
+    <t>Technology Partner</t>
+  </si>
+  <si>
+    <t>Customer - Channel</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -91,6 +285,20 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -119,14 +327,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -441,7 +652,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A25691F-935B-4F40-9036-DDC048F247EE}">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E1" sqref="E1:L1048576"/>
     </sheetView>
   </sheetViews>
@@ -512,4 +723,535 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72418A8C-8920-46A7-8BFB-1AD77E2B9F33}">
+  <dimension ref="A1:R6"/>
+  <sheetViews>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="6.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E2" t="s">
+        <v>36</v>
+      </c>
+      <c r="F2" t="s">
+        <v>37</v>
+      </c>
+      <c r="G2" t="s">
+        <v>38</v>
+      </c>
+      <c r="H2" t="s">
+        <v>52</v>
+      </c>
+      <c r="I2" t="s">
+        <v>46</v>
+      </c>
+      <c r="J2" t="s">
+        <v>41</v>
+      </c>
+      <c r="K2">
+        <v>4032</v>
+      </c>
+      <c r="L2" t="s">
+        <v>51</v>
+      </c>
+      <c r="M2" t="s">
+        <v>52</v>
+      </c>
+      <c r="N2" t="s">
+        <v>46</v>
+      </c>
+      <c r="O2" t="s">
+        <v>41</v>
+      </c>
+      <c r="P2">
+        <v>4032</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>51</v>
+      </c>
+      <c r="R2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>70</v>
+      </c>
+      <c r="B3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C3" t="s">
+        <v>66</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="E3" t="s">
+        <v>78</v>
+      </c>
+      <c r="F3" t="s">
+        <v>62</v>
+      </c>
+      <c r="G3" t="s">
+        <v>58</v>
+      </c>
+      <c r="H3" t="s">
+        <v>53</v>
+      </c>
+      <c r="I3" t="s">
+        <v>47</v>
+      </c>
+      <c r="J3" t="s">
+        <v>42</v>
+      </c>
+      <c r="K3">
+        <v>5600</v>
+      </c>
+      <c r="L3" t="s">
+        <v>51</v>
+      </c>
+      <c r="M3" t="s">
+        <v>53</v>
+      </c>
+      <c r="N3" t="s">
+        <v>47</v>
+      </c>
+      <c r="O3" t="s">
+        <v>42</v>
+      </c>
+      <c r="P3">
+        <v>5600</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>51</v>
+      </c>
+      <c r="R3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>72</v>
+      </c>
+      <c r="B4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C4" t="s">
+        <v>67</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="E4" t="s">
+        <v>79</v>
+      </c>
+      <c r="F4" t="s">
+        <v>37</v>
+      </c>
+      <c r="G4" t="s">
+        <v>59</v>
+      </c>
+      <c r="H4" t="s">
+        <v>54</v>
+      </c>
+      <c r="I4" t="s">
+        <v>48</v>
+      </c>
+      <c r="J4" t="s">
+        <v>43</v>
+      </c>
+      <c r="K4">
+        <v>6015</v>
+      </c>
+      <c r="L4" t="s">
+        <v>51</v>
+      </c>
+      <c r="M4" t="s">
+        <v>54</v>
+      </c>
+      <c r="N4" t="s">
+        <v>48</v>
+      </c>
+      <c r="O4" t="s">
+        <v>43</v>
+      </c>
+      <c r="P4">
+        <v>6015</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>51</v>
+      </c>
+      <c r="R4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>74</v>
+      </c>
+      <c r="B5" t="s">
+        <v>64</v>
+      </c>
+      <c r="C5" t="s">
+        <v>68</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="E5" t="s">
+        <v>63</v>
+      </c>
+      <c r="F5" t="s">
+        <v>62</v>
+      </c>
+      <c r="G5" t="s">
+        <v>60</v>
+      </c>
+      <c r="H5" t="s">
+        <v>55</v>
+      </c>
+      <c r="I5" t="s">
+        <v>49</v>
+      </c>
+      <c r="J5" t="s">
+        <v>44</v>
+      </c>
+      <c r="K5">
+        <v>1999</v>
+      </c>
+      <c r="L5" t="s">
+        <v>51</v>
+      </c>
+      <c r="M5" t="s">
+        <v>55</v>
+      </c>
+      <c r="N5" t="s">
+        <v>49</v>
+      </c>
+      <c r="O5" t="s">
+        <v>44</v>
+      </c>
+      <c r="P5">
+        <v>1999</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>51</v>
+      </c>
+      <c r="R5" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>76</v>
+      </c>
+      <c r="B6" t="s">
+        <v>65</v>
+      </c>
+      <c r="C6" t="s">
+        <v>69</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="E6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F6" t="s">
+        <v>63</v>
+      </c>
+      <c r="G6" t="s">
+        <v>61</v>
+      </c>
+      <c r="H6" t="s">
+        <v>56</v>
+      </c>
+      <c r="I6" t="s">
+        <v>50</v>
+      </c>
+      <c r="J6" t="s">
+        <v>45</v>
+      </c>
+      <c r="K6">
+        <v>2601</v>
+      </c>
+      <c r="L6" t="s">
+        <v>51</v>
+      </c>
+      <c r="M6" t="s">
+        <v>56</v>
+      </c>
+      <c r="N6" t="s">
+        <v>50</v>
+      </c>
+      <c r="O6" t="s">
+        <v>45</v>
+      </c>
+      <c r="P6">
+        <v>2601</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>51</v>
+      </c>
+      <c r="R6" t="s">
+        <v>57</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{A581C1E0-19D0-4121-883D-3549F6A653D5}"/>
+    <hyperlink ref="D3" r:id="rId2" xr:uid="{876E07BE-9DF5-493C-87CB-746754216B1D}"/>
+    <hyperlink ref="D4" r:id="rId3" xr:uid="{BA3668C0-0460-4E4A-9649-7F9E62AA37AF}"/>
+    <hyperlink ref="D5" r:id="rId4" xr:uid="{9FD03572-5937-459D-B05B-CA925019BD8E}"/>
+    <hyperlink ref="D6" r:id="rId5" xr:uid="{89DC3FF9-5E1E-4DDA-9F0E-2662CC82ADBC}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId6"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{095F3B76-D62F-4C9D-BBB0-E065067F0C6D}">
+  <dimension ref="A1:R2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="S1" sqref="S1:X1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="6.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E2" t="s">
+        <v>36</v>
+      </c>
+      <c r="F2" t="s">
+        <v>37</v>
+      </c>
+      <c r="G2" t="s">
+        <v>38</v>
+      </c>
+      <c r="H2" t="s">
+        <v>52</v>
+      </c>
+      <c r="I2" t="s">
+        <v>46</v>
+      </c>
+      <c r="J2" t="s">
+        <v>41</v>
+      </c>
+      <c r="K2">
+        <v>4032</v>
+      </c>
+      <c r="L2" t="s">
+        <v>51</v>
+      </c>
+      <c r="M2" t="s">
+        <v>52</v>
+      </c>
+      <c r="N2" t="s">
+        <v>46</v>
+      </c>
+      <c r="O2" t="s">
+        <v>41</v>
+      </c>
+      <c r="P2">
+        <v>4032</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>51</v>
+      </c>
+      <c r="R2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{422D1C9D-B7B6-40EB-B3C7-48A89029CA0A}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>